<commit_message>
se termino la matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Desarrollo/SVO/Documentos/Analisis y Diseño/SVO_MT.xlsx
+++ b/Desarrollo/SVO/Documentos/Analisis y Diseño/SVO_MT.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_Toc431294372" localSheetId="0">Hoja1!$A$20</definedName>
     <definedName name="_Toc498031000" localSheetId="0">Hoja1!$A$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
   <si>
     <t>Matriz de Trazabilidad de Casos de Uso vs. Requisitos</t>
   </si>
@@ -117,13 +118,82 @@
   </si>
   <si>
     <t>La matriz de trazabilidad nos ayuda a comprobar los casos de usos están cumpliendo con todos los requerimientos que ha solicitado el cliente; en la tabla siguiente, podemos visualizar que los casos de usos de nuestro sistema cumplen con los requisitos.</t>
+  </si>
+  <si>
+    <t>Matriz de Trazabilidad Casos de Uso vs Clases</t>
+  </si>
+  <si>
+    <t>CLASES</t>
+  </si>
+  <si>
+    <t>Leyenda:</t>
+  </si>
+  <si>
+    <t>1 - consultar</t>
+  </si>
+  <si>
+    <t>2 - insertar</t>
+  </si>
+  <si>
+    <t>3 - actualizar</t>
+  </si>
+  <si>
+    <t>4 - borrar</t>
+  </si>
+  <si>
+    <t>5 - todas</t>
+  </si>
+  <si>
+    <t>Pedido</t>
+  </si>
+  <si>
+    <t>ConsultarVenta</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>MantenerUsuario</t>
+  </si>
+  <si>
+    <t>HistorialVentas</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>UsuarioPerfil</t>
+  </si>
+  <si>
+    <t>CerrarSesión</t>
+  </si>
+  <si>
+    <t>IniciarSesion</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Sede</t>
+  </si>
+  <si>
+    <t>MantenerProductos</t>
+  </si>
+  <si>
+    <t>La matriz de trazabilidad casos de uso vs clases nos ayuda a relacionarlos de tal manera que se puede conocer qué clase deriva de qué caso de uso; en la tabla siguiente, podemos visualizar como los casos de usos de nuestro sistema se relacionan con las clases.</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>1,3,4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,13 +217,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -167,6 +230,23 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -266,34 +346,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -577,16 +707,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R17"/>
+  <dimension ref="A2:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -603,350 +739,683 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="8"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="D9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R10" s="3"/>
+      <c r="D10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="10"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="D11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R12" s="3"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="10"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R14" s="3"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="10"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="6" t="s">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R17" s="3"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="10"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D24" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10">
+        <v>1</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10">
+        <v>1</v>
+      </c>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10">
+        <v>1</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10">
+        <v>1</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10">
+        <v>2</v>
+      </c>
+      <c r="J28" s="10">
+        <v>2</v>
+      </c>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10">
+        <v>2</v>
+      </c>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10">
+        <v>2</v>
+      </c>
+      <c r="F32" s="10">
+        <v>2</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10">
+        <v>2</v>
+      </c>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10">
+        <v>1</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10">
+        <v>1</v>
+      </c>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10">
+        <v>1</v>
+      </c>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10">
+        <v>2</v>
+      </c>
+      <c r="O35" s="10"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="15"/>
+      <c r="D38" s="16"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="16"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
     <mergeCell ref="D6:R6"/>
     <mergeCell ref="B8:B17"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="D24:O24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>